<commit_message>
Actualizar porcentajes en la calculadora de presupuesto Excel
Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Calculadora de presupuesto.xlsx
+++ b/Calculadora de presupuesto.xlsx
@@ -10,7 +10,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="VuEwI3uOLVBA/Y4LEBjPesG239sNjG/wGIhnERF5QMU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="EGJdHiBrwvrV/9iyG9GNIpWDDhsUPPmjFZw0TZQjU6A="/>
     </ext>
   </extLst>
 </workbook>
@@ -31,7 +31,7 @@
     <t>Otros productos</t>
   </si>
   <si>
-    <t>Precio sin IVA</t>
+    <t>Precio s/IVA</t>
   </si>
   <si>
     <t>Croissant</t>
@@ -122,17 +122,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <b/>
       <sz val="13.0"/>
@@ -178,14 +178,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFD9D9D9"/>
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor rgb="FFC9DAF8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC9DAF8"/>
-        <bgColor rgb="FFC9DAF8"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -276,34 +276,37 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="6" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="6" fillId="0" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
@@ -317,7 +320,7 @@
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -331,13 +334,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -570,928 +576,908 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="17.88"/>
-    <col customWidth="1" min="5" max="5" width="21.25"/>
+    <col customWidth="1" min="3" max="3" width="19.88"/>
+    <col customWidth="1" min="4" max="4" width="13.75"/>
+    <col customWidth="1" min="5" max="5" width="13.63"/>
     <col customWidth="1" min="6" max="6" width="14.5"/>
     <col customWidth="1" min="7" max="7" width="18.25"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" ht="24.0" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+    <row r="1" ht="22.5" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-    </row>
-    <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="5" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" ht="21.0" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="6" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+    </row>
+    <row r="4" ht="25.5" customHeight="1">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7">
-        <f>IFERROR(VLOOKUP(C6, 'Lista de precios'!C:F, 4, FALSE), "")</f>
-        <v>4.950413223</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9">
-        <f t="shared" ref="G6:G21" si="1">F6 / (1 + 21%)</f>
+      <c r="B4" s="8">
+        <f>IFERROR(VLOOKUP(A4, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+        <v>5.445454545</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10">
+        <f t="shared" ref="E4:E19" si="1">D4 / (1 + 10%)</f>
         <v>0</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="6" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7">
-        <f>IFERROR(VLOOKUP(C7, 'Lista de precios'!C:F, 4, FALSE), "")</f>
-        <v>7.429752066</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9">
+      <c r="B5" s="8">
+        <f>IFERROR(VLOOKUP(A5, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+        <v>8.172727273</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="7">
-        <f>IFERROR(VLOOKUP(C8, 'Lista de precios'!C:F, 4, FALSE), "")</f>
-        <v>6.603305785</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="9">
+      <c r="B6" s="8">
+        <f>IFERROR(VLOOKUP(A6, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+        <v>7.263636364</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="6" t="s">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="7">
-        <f>IFERROR(VLOOKUP(C9, 'Lista de precios'!C:F, 4, FALSE), "")</f>
-        <v>7.429752066</v>
-      </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9">
+      <c r="B7" s="8">
+        <f>IFERROR(VLOOKUP(A7, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+        <v>8.172727273</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="6" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7">
-        <f>IFERROR(VLOOKUP(C10, 'Lista de precios'!C:F, 4, FALSE), "")</f>
-        <v>3.876033058</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="9">
+      <c r="B8" s="8">
+        <f>IFERROR(VLOOKUP(A8, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+        <v>4.263636364</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="6" t="s">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7">
-        <f>IFERROR(VLOOKUP(C11, 'Lista de precios'!C:F, 4, FALSE), "")</f>
-        <v>2.223140496</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="9">
+      <c r="B9" s="8">
+        <f>IFERROR(VLOOKUP(A9, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+        <v>2.445454545</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="6" t="s">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="7">
-        <f>IFERROR(VLOOKUP(C12, 'Lista de precios'!C:F, 4, FALSE), "")</f>
-        <v>9.082644628</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="9">
+      <c r="B10" s="8">
+        <f>IFERROR(VLOOKUP(A10, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+        <v>9.990909091</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C13, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="14"/>
+      <c r="B11" s="8" t="str">
+        <f>IFERROR(VLOOKUP(A11, 'Lista de precios'!C:F, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="9">
+      <c r="C11" s="12"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C14, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8" t="str">
+        <f>IFERROR(VLOOKUP(A12, 'Lista de precios'!C:F, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="9">
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C15, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="14"/>
+      <c r="B13" s="8" t="str">
+        <f>IFERROR(VLOOKUP(A13, 'Lista de precios'!C:F, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="9">
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C16, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="14"/>
+      <c r="B14" s="8" t="str">
+        <f>IFERROR(VLOOKUP(A14, 'Lista de precios'!C:F, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="9">
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C17, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="14"/>
+      <c r="B15" s="8" t="str">
+        <f>IFERROR(VLOOKUP(A15, 'Lista de precios'!C:F, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="9">
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C18, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="14"/>
+      <c r="B16" s="8" t="str">
+        <f>IFERROR(VLOOKUP(A16, 'Lista de precios'!C:F, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="9">
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C19, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="14"/>
+      <c r="B17" s="8" t="str">
+        <f>IFERROR(VLOOKUP(A17, 'Lista de precios'!C:F, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="9">
+      <c r="C17" s="12"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="7" t="str">
-        <f>IFERROR(VLOOKUP(C20, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="14"/>
+      <c r="B18" s="8" t="str">
+        <f>IFERROR(VLOOKUP(A18, 'Lista de precios'!C:F, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="9">
+      <c r="C18" s="12"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15" t="str">
-        <f>IFERROR(VLOOKUP(C21, 'Lista de precios'!C:F, 4, FALSE), "")</f>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16" t="str">
+        <f>IFERROR(VLOOKUP(A19, 'Lista de precios'!C:F, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="9">
+      <c r="C19" s="17"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+    </row>
+    <row r="20" ht="17.25" customHeight="1">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+    </row>
+    <row r="21" ht="22.5" customHeight="1">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="20">
+        <v>40.0</v>
+      </c>
+      <c r="E21" s="21">
+        <f>SUM(B4:B19,E4:E19)</f>
+        <v>45.75454545</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
     </row>
     <row r="22" ht="22.5" customHeight="1">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-    </row>
-    <row r="23" ht="22.5" customHeight="1">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="19">
-        <v>40.0</v>
-      </c>
-      <c r="G23" s="20">
-        <f>SUM(D6:D21,G6:G21)</f>
-        <v>41.59504132</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-    </row>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
@@ -2453,23 +2439,22 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G23">
+  <conditionalFormatting sqref="E21">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>G23&gt;F23</formula>
+      <formula>E21&gt;D21</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G23">
+  <conditionalFormatting sqref="E21">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>G23&gt;F23</formula>
+      <formula>E21&gt;D21</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C6:C21">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A4:A19">
       <formula1>"Arándanos,Berlinas,Bizcocho,Cookies,Crodots,Croissant,Empanada,Frambuesas,Galletas cuadradas,Mandarinas,Manzanas rojas,Manzanas verdes,Muffins,Naranjas,Pan,Plátanos,Tortillas,Trenza,Zumo Caribe,Zumo naranja "</formula1>
     </dataValidation>
   </dataValidations>
@@ -2492,925 +2477,925 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="C1" s="21"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="C2" s="21"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="C3" s="21"/>
+      <c r="C3" s="22"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="24">
         <v>8.99</v>
       </c>
-      <c r="E5" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F5" s="23">
+      <c r="E5" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="24">
         <f t="shared" ref="F5:F25" si="1">D5 / (1 + E5)</f>
-        <v>7.429752066</v>
+        <v>8.172727273</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="24">
         <v>8.99</v>
       </c>
-      <c r="E6" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F6" s="23">
+      <c r="E6" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="24">
         <f t="shared" si="1"/>
-        <v>7.429752066</v>
+        <v>8.172727273</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="24">
         <v>7.99</v>
       </c>
-      <c r="E7" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F7" s="23">
+      <c r="E7" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="24">
         <f t="shared" si="1"/>
-        <v>6.603305785</v>
+        <v>7.263636364</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="24">
         <v>3.99</v>
       </c>
-      <c r="E8" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F8" s="23">
+      <c r="E8" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="24">
         <f t="shared" si="1"/>
-        <v>3.297520661</v>
+        <v>3.627272727</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="26">
         <v>1.99</v>
       </c>
-      <c r="E9" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F9" s="23">
+      <c r="E9" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="24">
         <f t="shared" si="1"/>
-        <v>1.644628099</v>
+        <v>1.809090909</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="24">
         <v>10.99</v>
       </c>
-      <c r="E10" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F10" s="23">
+      <c r="E10" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F10" s="24">
         <f t="shared" si="1"/>
-        <v>9.082644628</v>
+        <v>9.990909091</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="26">
         <v>11.49</v>
       </c>
-      <c r="E11" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F11" s="23">
+      <c r="E11" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="24">
         <f t="shared" si="1"/>
-        <v>9.495867769</v>
+        <v>10.44545455</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="26">
         <v>4.69</v>
       </c>
-      <c r="E12" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F12" s="23">
+      <c r="E12" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="24">
         <f t="shared" si="1"/>
-        <v>3.876033058</v>
+        <v>4.263636364</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="24">
         <v>5.49</v>
       </c>
-      <c r="E13" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F13" s="23">
+      <c r="E13" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="24">
         <f t="shared" si="1"/>
-        <v>4.537190083</v>
+        <v>4.990909091</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="24">
         <v>2.69</v>
       </c>
-      <c r="E14" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F14" s="23">
+      <c r="E14" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="24">
         <f t="shared" si="1"/>
-        <v>2.223140496</v>
+        <v>2.445454545</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="24">
         <v>1.89</v>
       </c>
-      <c r="E15" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F15" s="23">
+      <c r="E15" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="24">
         <f t="shared" si="1"/>
-        <v>1.561983471</v>
+        <v>1.718181818</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="26">
         <v>4.69</v>
       </c>
-      <c r="E16" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F16" s="23">
+      <c r="E16" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F16" s="24">
         <f t="shared" si="1"/>
-        <v>3.876033058</v>
+        <v>4.263636364</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="26">
         <v>5.89</v>
       </c>
-      <c r="E17" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F17" s="23">
+      <c r="E17" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F17" s="24">
         <f t="shared" si="1"/>
-        <v>4.867768595</v>
+        <v>5.354545455</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="26">
         <v>6.49</v>
       </c>
-      <c r="E18" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F18" s="23">
+      <c r="E18" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="24">
         <f t="shared" si="1"/>
-        <v>5.363636364</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="26">
         <v>6.99</v>
       </c>
-      <c r="E19" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F19" s="23">
+      <c r="E19" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="24">
         <f t="shared" si="1"/>
-        <v>5.776859504</v>
+        <v>6.354545455</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="26">
         <v>9.99</v>
       </c>
-      <c r="E20" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F20" s="23">
+      <c r="E20" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F20" s="24">
         <f t="shared" si="1"/>
-        <v>8.256198347</v>
+        <v>9.081818182</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="26">
         <v>9.99</v>
       </c>
-      <c r="E21" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F21" s="23">
+      <c r="E21" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="24">
         <f t="shared" si="1"/>
-        <v>8.256198347</v>
+        <v>9.081818182</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="26">
         <v>5.99</v>
       </c>
-      <c r="E22" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F22" s="23">
+      <c r="E22" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F22" s="24">
         <f t="shared" si="1"/>
-        <v>4.950413223</v>
+        <v>5.445454545</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="26">
         <v>6.29</v>
       </c>
-      <c r="E23" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F23" s="23">
+      <c r="E23" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F23" s="24">
         <f t="shared" si="1"/>
-        <v>5.198347107</v>
+        <v>5.718181818</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="26">
         <v>9.99</v>
       </c>
-      <c r="E24" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F24" s="23">
+      <c r="E24" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F24" s="24">
         <f t="shared" si="1"/>
-        <v>8.256198347</v>
+        <v>9.081818182</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="24">
         <v>8.99</v>
       </c>
-      <c r="E25" s="24">
-        <v>0.21</v>
-      </c>
-      <c r="F25" s="23">
+      <c r="E25" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F25" s="24">
         <f t="shared" si="1"/>
-        <v>7.429752066</v>
+        <v>8.172727273</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="C26" s="26"/>
+      <c r="C26" s="27"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="C27" s="21"/>
+      <c r="C27" s="22"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="C28" s="21"/>
-      <c r="E28" s="24"/>
+      <c r="C28" s="22"/>
+      <c r="E28" s="28"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="C29" s="21"/>
+      <c r="C29" s="22"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="21"/>
+      <c r="C30" s="22"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="21"/>
+      <c r="C31" s="22"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="21"/>
+      <c r="C32" s="22"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="21"/>
+      <c r="C33" s="22"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="21"/>
+      <c r="C34" s="22"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="21"/>
+      <c r="C35" s="22"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="21"/>
+      <c r="C36" s="22"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="21"/>
+      <c r="C37" s="22"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="21"/>
+      <c r="C38" s="22"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="21"/>
+      <c r="C39" s="22"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="21"/>
+      <c r="C40" s="22"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="21"/>
+      <c r="C41" s="22"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="21"/>
+      <c r="C42" s="22"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="21"/>
+      <c r="C43" s="22"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="21"/>
+      <c r="C44" s="22"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="21"/>
+      <c r="C45" s="22"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="21"/>
+      <c r="C46" s="22"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="21"/>
+      <c r="C47" s="22"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="21"/>
+      <c r="C48" s="22"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="21"/>
+      <c r="C49" s="22"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="21"/>
+      <c r="C50" s="22"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="21"/>
+      <c r="C51" s="22"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="21"/>
+      <c r="C52" s="22"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="21"/>
+      <c r="C53" s="22"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="21"/>
+      <c r="C54" s="22"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="21"/>
+      <c r="C55" s="22"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="21"/>
+      <c r="C56" s="22"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="21"/>
+      <c r="C57" s="22"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="21"/>
+      <c r="C58" s="22"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="21"/>
+      <c r="C59" s="22"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="21"/>
+      <c r="C60" s="22"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="21"/>
+      <c r="C61" s="22"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="21"/>
+      <c r="C62" s="22"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="21"/>
+      <c r="C63" s="22"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="21"/>
+      <c r="C64" s="22"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="21"/>
+      <c r="C65" s="22"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="21"/>
+      <c r="C66" s="22"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="21"/>
+      <c r="C67" s="22"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="21"/>
+      <c r="C68" s="22"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="21"/>
+      <c r="C69" s="22"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="21"/>
+      <c r="C70" s="22"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="21"/>
+      <c r="C71" s="22"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="21"/>
+      <c r="C72" s="22"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="21"/>
+      <c r="C73" s="22"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="21"/>
+      <c r="C74" s="22"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="21"/>
+      <c r="C75" s="22"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="C76" s="21"/>
+      <c r="C76" s="22"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="C77" s="21"/>
+      <c r="C77" s="22"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="C78" s="21"/>
+      <c r="C78" s="22"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="21"/>
+      <c r="C79" s="22"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="C80" s="21"/>
+      <c r="C80" s="22"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="C81" s="21"/>
+      <c r="C81" s="22"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="C82" s="21"/>
+      <c r="C82" s="22"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="21"/>
+      <c r="C83" s="22"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="C84" s="21"/>
+      <c r="C84" s="22"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="C85" s="21"/>
+      <c r="C85" s="22"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="C86" s="21"/>
+      <c r="C86" s="22"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="C87" s="21"/>
+      <c r="C87" s="22"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="C88" s="21"/>
+      <c r="C88" s="22"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="C89" s="21"/>
+      <c r="C89" s="22"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="21"/>
+      <c r="C90" s="22"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="21"/>
+      <c r="C91" s="22"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="C92" s="21"/>
+      <c r="C92" s="22"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="21"/>
+      <c r="C93" s="22"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="21"/>
+      <c r="C94" s="22"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="21"/>
+      <c r="C95" s="22"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="21"/>
+      <c r="C96" s="22"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="21"/>
+      <c r="C97" s="22"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="21"/>
+      <c r="C98" s="22"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="21"/>
+      <c r="C99" s="22"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="21"/>
+      <c r="C100" s="22"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="21"/>
+      <c r="C101" s="22"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="21"/>
+      <c r="C102" s="22"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="21"/>
+      <c r="C103" s="22"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="21"/>
+      <c r="C104" s="22"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="21"/>
+      <c r="C105" s="22"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="21"/>
+      <c r="C106" s="22"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="21"/>
+      <c r="C107" s="22"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="21"/>
+      <c r="C108" s="22"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="21"/>
+      <c r="C109" s="22"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="21"/>
+      <c r="C110" s="22"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="21"/>
+      <c r="C111" s="22"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="21"/>
+      <c r="C112" s="22"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="21"/>
+      <c r="C113" s="22"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="21"/>
+      <c r="C114" s="22"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="21"/>
+      <c r="C115" s="22"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="21"/>
+      <c r="C116" s="22"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="21"/>
+      <c r="C117" s="22"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="21"/>
+      <c r="C118" s="22"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="21"/>
+      <c r="C119" s="22"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="21"/>
+      <c r="C120" s="22"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="21"/>
+      <c r="C121" s="22"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="21"/>
+      <c r="C122" s="22"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="21"/>
+      <c r="C123" s="22"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="21"/>
+      <c r="C124" s="22"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="21"/>
+      <c r="C125" s="22"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="21"/>
+      <c r="C126" s="22"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="21"/>
+      <c r="C127" s="22"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="21"/>
+      <c r="C128" s="22"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="C129" s="21"/>
+      <c r="C129" s="22"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="C130" s="21"/>
+      <c r="C130" s="22"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="21"/>
+      <c r="C131" s="22"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="21"/>
+      <c r="C132" s="22"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="21"/>
+      <c r="C133" s="22"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="21"/>
+      <c r="C134" s="22"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="21"/>
+      <c r="C135" s="22"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="21"/>
+      <c r="C136" s="22"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="21"/>
+      <c r="C137" s="22"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="21"/>
+      <c r="C138" s="22"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="21"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="21"/>
+      <c r="C140" s="22"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="21"/>
+      <c r="C141" s="22"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="21"/>
+      <c r="C142" s="22"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="21"/>
+      <c r="C143" s="22"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="21"/>
+      <c r="C144" s="22"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="21"/>
+      <c r="C145" s="22"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="21"/>
+      <c r="C146" s="22"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="21"/>
+      <c r="C147" s="22"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="21"/>
+      <c r="C148" s="22"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="21"/>
+      <c r="C149" s="22"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="21"/>
+      <c r="C150" s="22"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="21"/>
+      <c r="C151" s="22"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="21"/>
+      <c r="C152" s="22"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="21"/>
+      <c r="C153" s="22"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="21"/>
+      <c r="C154" s="22"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="21"/>
+      <c r="C155" s="22"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="21"/>
+      <c r="C156" s="22"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="21"/>
+      <c r="C157" s="22"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="21"/>
+      <c r="C158" s="22"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="21"/>
+      <c r="C159" s="22"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="21"/>
+      <c r="C160" s="22"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="21"/>
+      <c r="C161" s="22"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="21"/>
+      <c r="C162" s="22"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="C163" s="21"/>
+      <c r="C163" s="22"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="C164" s="21"/>
+      <c r="C164" s="22"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="C165" s="21"/>
+      <c r="C165" s="22"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="C166" s="21"/>
+      <c r="C166" s="22"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="C167" s="21"/>
+      <c r="C167" s="22"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="C168" s="21"/>
+      <c r="C168" s="22"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="C169" s="21"/>
+      <c r="C169" s="22"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="C170" s="21"/>
+      <c r="C170" s="22"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="C171" s="21"/>
+      <c r="C171" s="22"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="C172" s="21"/>
+      <c r="C172" s="22"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="C173" s="21"/>
+      <c r="C173" s="22"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="C174" s="21"/>
+      <c r="C174" s="22"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="C175" s="21"/>
+      <c r="C175" s="22"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="C176" s="21"/>
+      <c r="C176" s="22"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="C177" s="21"/>
+      <c r="C177" s="22"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="C178" s="21"/>
+      <c r="C178" s="22"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="C179" s="21"/>
+      <c r="C179" s="22"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="C180" s="21"/>
+      <c r="C180" s="22"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="C181" s="21"/>
+      <c r="C181" s="22"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="C182" s="21"/>
+      <c r="C182" s="22"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="C183" s="21"/>
+      <c r="C183" s="22"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="C184" s="21"/>
+      <c r="C184" s="22"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="C185" s="21"/>
+      <c r="C185" s="22"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="C186" s="21"/>
+      <c r="C186" s="22"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="C187" s="21"/>
+      <c r="C187" s="22"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="C188" s="21"/>
+      <c r="C188" s="22"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="C189" s="21"/>
+      <c r="C189" s="22"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="C190" s="21"/>
+      <c r="C190" s="22"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="C191" s="21"/>
+      <c r="C191" s="22"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="C192" s="21"/>
+      <c r="C192" s="22"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="C193" s="21"/>
+      <c r="C193" s="22"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="C194" s="21"/>
+      <c r="C194" s="22"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="C195" s="21"/>
+      <c r="C195" s="22"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="C196" s="21"/>
+      <c r="C196" s="22"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="C197" s="21"/>
+      <c r="C197" s="22"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="C198" s="21"/>
+      <c r="C198" s="22"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="C199" s="21"/>
+      <c r="C199" s="22"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="C200" s="21"/>
+      <c r="C200" s="22"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="C201" s="21"/>
+      <c r="C201" s="22"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="C202" s="21"/>
+      <c r="C202" s="22"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="C203" s="21"/>
+      <c r="C203" s="22"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="C204" s="21"/>
+      <c r="C204" s="22"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="C205" s="21"/>
+      <c r="C205" s="22"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="C206" s="21"/>
+      <c r="C206" s="22"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="C207" s="21"/>
+      <c r="C207" s="22"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="C208" s="21"/>
+      <c r="C208" s="22"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="C209" s="21"/>
+      <c r="C209" s="22"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="C210" s="21"/>
+      <c r="C210" s="22"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="C211" s="21"/>
+      <c r="C211" s="22"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="C212" s="21"/>
+      <c r="C212" s="22"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="C213" s="21"/>
+      <c r="C213" s="22"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="C214" s="21"/>
+      <c r="C214" s="22"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="C215" s="21"/>
+      <c r="C215" s="22"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="C216" s="21"/>
+      <c r="C216" s="22"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="C217" s="21"/>
+      <c r="C217" s="22"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="C218" s="21"/>
+      <c r="C218" s="22"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="C219" s="21"/>
+      <c r="C219" s="22"/>
     </row>
     <row r="220" ht="15.75" customHeight="1"/>
     <row r="221" ht="15.75" customHeight="1"/>

</xml_diff>